<commit_message>
Arduino Uno led3.ino 追加 LED点灯のきほん
</commit_message>
<xml_diff>
--- a/PIN.xlsx
+++ b/PIN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiga\denden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CE7286-D8DD-4515-BEAE-C5D205EBA2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F271CD7-2BD9-4A26-8824-3B757B777401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2990" yWindow="3150" windowWidth="31810" windowHeight="16950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,6 +171,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>283680</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E4BB90B-0BA4-85BC-DF99-B1EFC5FB77B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="8642350"/>
+          <a:ext cx="5452580" cy="3854450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -439,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>